<commit_message>
Updating Tile Colection Organizer
</commit_message>
<xml_diff>
--- a/Excel/Tile Colection.xlsx
+++ b/Excel/Tile Colection.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Photonic\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Photonic\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="16">
-  <si>
-    <t>lvl</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>01-Curva-Esq-01</t>
   </si>
@@ -68,18 +65,41 @@
     <t>03-Expiral-02</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Juntas Testadas?</t>
+  </si>
+  <si>
+    <t># de aparições</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>lvl 1</t>
+  </si>
+  <si>
+    <t>lvl 2</t>
+  </si>
+  <si>
+    <t>lvl 3</t>
+  </si>
+  <si>
+    <t>lvl 4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -122,13 +142,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,241 +469,262 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G16"/>
+  <dimension ref="B2:H17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="3.140625" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="3.28515625" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="1"/>
-      <c r="C2" s="1" t="s">
+    <row r="2" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2">
+        <v>3</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2">
+        <v>2</v>
+      </c>
+      <c r="E5" s="2">
+        <v>2</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+      <c r="D6" s="2">
+        <v>2</v>
+      </c>
+      <c r="E6" s="2">
+        <v>2</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2">
+        <v>3</v>
+      </c>
+      <c r="G7" s="2">
+        <v>1</v>
+      </c>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2">
+        <v>1</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1</v>
+      </c>
+      <c r="G8" s="2">
+        <v>2</v>
+      </c>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2">
+        <v>1</v>
+      </c>
+      <c r="G9" s="2">
+        <v>1</v>
+      </c>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2">
+        <v>2</v>
+      </c>
+      <c r="G10" s="2">
+        <v>1</v>
+      </c>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1</v>
+      </c>
+      <c r="F11" s="2">
+        <v>4</v>
+      </c>
+      <c r="G11" s="2">
+        <v>5</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2">
-        <v>2</v>
-      </c>
-      <c r="E3" s="2">
+      <c r="D12" s="2"/>
+      <c r="E12" s="2">
+        <v>1</v>
+      </c>
+      <c r="F12" s="2">
+        <v>4</v>
+      </c>
+      <c r="G12" s="2">
         <v>3</v>
       </c>
-      <c r="F3" s="2">
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2">
+        <v>2</v>
+      </c>
+      <c r="G13" s="2">
         <v>4</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="1"/>
-      <c r="C15" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2">
+        <v>2</v>
+      </c>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C15" s="1"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="1"/>
-      <c r="C16" s="2"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C16" s="1"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="4">
+        <f>COUNTA(C4:C16)</f>
+        <v>11</v>
+      </c>
+      <c r="D17" s="4">
+        <f t="shared" ref="D17:F17" si="0">SUM(D4:D16)</f>
+        <v>7</v>
+      </c>
+      <c r="E17" s="4">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="F17" s="4">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="G17" s="4">
+        <f>SUM(G4:G16)</f>
+        <v>19</v>
+      </c>
+      <c r="H17" s="4">
+        <f>COUNTA(H4:H16)</f>
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Still fixing conection between tiles
</commit_message>
<xml_diff>
--- a/Excel/Tile Colection.xlsx
+++ b/Excel/Tile Colection.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>01-Curva-Esq-01</t>
   </si>
@@ -472,7 +472,7 @@
   <dimension ref="B2:H17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,9 +552,7 @@
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="H6" s="2"/>
     </row>
     <row r="7" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
@@ -570,7 +568,9 @@
       <c r="G7" s="2">
         <v>1</v>
       </c>
-      <c r="H7" s="2"/>
+      <c r="H7" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="8" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
@@ -586,7 +586,9 @@
       <c r="G8" s="2">
         <v>2</v>
       </c>
-      <c r="H8" s="2"/>
+      <c r="H8" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="9" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
@@ -600,7 +602,9 @@
       <c r="G9" s="2">
         <v>1</v>
       </c>
-      <c r="H9" s="2"/>
+      <c r="H9" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="10" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
@@ -720,7 +724,7 @@
       </c>
       <c r="H17" s="4">
         <f>COUNTA(H4:H16)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add 02-Narrow-01. Renamed 04-Narrow to 03-Narrow. Edited level 2/3/4 tile collection. Edited Excel
</commit_message>
<xml_diff>
--- a/Excel/Tile Colection.xlsx
+++ b/Excel/Tile Colection.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Photonic\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Game Design\Unreal Projects\Photonic\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
   <si>
     <t>01-Curva-Esq-01</t>
   </si>
@@ -84,6 +84,12 @@
   </si>
   <si>
     <t>lvl 4</t>
+  </si>
+  <si>
+    <t>02-Narrow-01</t>
+  </si>
+  <si>
+    <t>03-Narrow-01</t>
   </si>
 </sst>
 </file>
@@ -472,7 +478,7 @@
   <dimension ref="B2:H17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,7 +522,7 @@
         <v>2</v>
       </c>
       <c r="E4" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -532,7 +538,7 @@
         <v>2</v>
       </c>
       <c r="E5" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -548,7 +554,7 @@
         <v>2</v>
       </c>
       <c r="E6" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -626,37 +632,33 @@
     </row>
     <row r="11" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2">
         <v>3</v>
       </c>
-      <c r="D11" s="2">
-        <v>1</v>
-      </c>
-      <c r="E11" s="2">
-        <v>1</v>
-      </c>
-      <c r="F11" s="2">
-        <v>4</v>
-      </c>
-      <c r="G11" s="2">
-        <v>5</v>
-      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
       <c r="H11" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="12" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="2"/>
+        <v>3</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
       <c r="E12" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F12" s="2">
         <v>4</v>
       </c>
       <c r="G12" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>4</v>
@@ -664,15 +666,17 @@
     </row>
     <row r="13" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="E13" s="2">
+        <v>1</v>
+      </c>
       <c r="F13" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G13" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>4</v>
@@ -680,32 +684,46 @@
     </row>
     <row r="14" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="F14" s="2">
+        <v>2</v>
+      </c>
       <c r="G14" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="15" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C15" s="1"/>
+      <c r="C15" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
+      <c r="G15" s="2">
+        <v>2</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="16" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C16" s="1"/>
+      <c r="C16" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
+      <c r="F16" s="2">
+        <v>3</v>
+      </c>
+      <c r="G16" s="2">
+        <v>1</v>
+      </c>
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
@@ -714,7 +732,7 @@
       </c>
       <c r="C17" s="4">
         <f>COUNTA(C4:C16)</f>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D17" s="4">
         <f t="shared" ref="D17:F17" si="0">SUM(D4:D16)</f>
@@ -722,19 +740,19 @@
       </c>
       <c r="E17" s="4">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F17" s="4">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G17" s="4">
         <f>SUM(G4:G16)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H17" s="4">
         <f>COUNTA(H4:H16)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pente fino nas juntas do loop 2
</commit_message>
<xml_diff>
--- a/Excel/Tile Colection.xlsx
+++ b/Excel/Tile Colection.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
   <si>
     <t>01-Curva-Esq-01</t>
   </si>
@@ -481,7 +481,7 @@
   <dimension ref="B2:H18"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -737,7 +737,9 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
+      <c r="H17" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
@@ -765,7 +767,7 @@
       </c>
       <c r="H18" s="4">
         <f>COUNTA(H4:H17)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
01_Curva_Cima_01 Implemented and Tested
</commit_message>
<xml_diff>
--- a/Excel/Tile Colection.xlsx
+++ b/Excel/Tile Colection.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
   <si>
     <t>01-Curva-Esq-01</t>
   </si>
@@ -93,13 +93,19 @@
   </si>
   <si>
     <t>BP_Loop-01</t>
+  </si>
+  <si>
+    <t>BP_Curva_Cima_01</t>
+  </si>
+  <si>
+    <t>BP_Loop-01 Não buga com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,13 +121,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -151,7 +170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -161,8 +180,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -478,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H18"/>
+  <dimension ref="B2:I19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,285 +518,339 @@
     <col min="1" max="1" width="4.7109375" customWidth="1"/>
     <col min="3" max="3" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="7" width="3.28515625" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D2" t="s">
+    <row r="2" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D2" s="6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+    </row>
+    <row r="3" spans="3:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="2">
-        <v>2</v>
-      </c>
-      <c r="E4" s="2">
-        <v>2</v>
-      </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+      <c r="D4" s="8">
+        <v>2</v>
+      </c>
+      <c r="E4" s="8">
+        <v>2</v>
+      </c>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
       <c r="H4" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="2">
-        <v>2</v>
-      </c>
-      <c r="E5" s="2">
+      <c r="D5" s="8">
+        <v>2</v>
+      </c>
+      <c r="E5" s="8">
         <v>3</v>
       </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
       <c r="H5" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="2">
-        <v>2</v>
-      </c>
-      <c r="E6" s="2">
+      <c r="D6" s="8">
+        <v>2</v>
+      </c>
+      <c r="E6" s="8">
         <v>3</v>
       </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
       <c r="H6" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2">
-        <v>1</v>
-      </c>
-      <c r="F7" s="2">
+      <c r="D8" s="8"/>
+      <c r="E8" s="8">
+        <v>1</v>
+      </c>
+      <c r="F8" s="8">
         <v>3</v>
       </c>
-      <c r="G7" s="2">
-        <v>1</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C8" s="1" t="s">
+      <c r="G8" s="8">
+        <v>1</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2">
-        <v>1</v>
-      </c>
-      <c r="F8" s="2">
-        <v>1</v>
-      </c>
-      <c r="G8" s="2">
-        <v>2</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="8"/>
+      <c r="E9" s="8">
+        <v>1</v>
+      </c>
+      <c r="F9" s="8">
+        <v>1</v>
+      </c>
+      <c r="G9" s="8">
+        <v>2</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2">
-        <v>1</v>
-      </c>
-      <c r="G9" s="2">
-        <v>1</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8">
+        <v>1</v>
+      </c>
+      <c r="G10" s="8">
+        <v>1</v>
+      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2">
-        <v>2</v>
-      </c>
-      <c r="G10" s="2">
-        <v>1</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8">
+        <v>2</v>
+      </c>
+      <c r="G11" s="8">
+        <v>1</v>
+      </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2">
+      <c r="D12" s="8"/>
+      <c r="E12" s="8">
         <v>3</v>
       </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C12" s="1" t="s">
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C13" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="2">
-        <v>1</v>
-      </c>
-      <c r="E12" s="2">
-        <v>2</v>
-      </c>
-      <c r="F12" s="2">
-        <v>4</v>
-      </c>
-      <c r="G12" s="2">
+      <c r="D13" s="8">
+        <v>1</v>
+      </c>
+      <c r="E13" s="8">
+        <v>2</v>
+      </c>
+      <c r="F13" s="8">
+        <v>4</v>
+      </c>
+      <c r="G13" s="8">
         <v>5</v>
       </c>
-      <c r="H12" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C13" s="1" t="s">
+      <c r="H13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2">
-        <v>1</v>
-      </c>
-      <c r="F13" s="2">
-        <v>4</v>
-      </c>
-      <c r="G13" s="2">
+      <c r="D14" s="8"/>
+      <c r="E14" s="8">
+        <v>1</v>
+      </c>
+      <c r="F14" s="8">
+        <v>4</v>
+      </c>
+      <c r="G14" s="8">
         <v>3</v>
       </c>
-      <c r="H13" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C14" s="1" t="s">
+      <c r="H14" s="2"/>
+      <c r="I14" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2">
-        <v>2</v>
-      </c>
-      <c r="G14" s="2">
-        <v>4</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8">
+        <v>2</v>
+      </c>
+      <c r="G15" s="8">
+        <v>4</v>
+      </c>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2">
-        <v>2</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8">
+        <v>2</v>
+      </c>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2">
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8">
         <v>3</v>
       </c>
-      <c r="G16" s="2">
-        <v>1</v>
-      </c>
-      <c r="H16" s="2"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C17" s="1" t="s">
+      <c r="G17" s="8">
+        <v>1</v>
+      </c>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C18" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="3" t="s">
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="4">
-        <f>COUNTA(C4:C17)</f>
-        <v>14</v>
-      </c>
-      <c r="D18" s="4">
-        <f t="shared" ref="D18:F18" si="0">SUM(D4:D17)</f>
+      <c r="C19" s="4">
+        <f>COUNTA(C4:C18)</f>
+        <v>15</v>
+      </c>
+      <c r="D19" s="9">
+        <f t="shared" ref="D19:F19" si="0">SUM(D4:D18)</f>
         <v>7</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E19" s="9">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F19" s="9">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="G18" s="4">
-        <f>SUM(G4:G17)</f>
+      <c r="G19" s="9">
+        <f>SUM(G4:G18)</f>
         <v>20</v>
       </c>
-      <c r="H18" s="4">
-        <f>COUNTA(H4:H17)</f>
-        <v>13</v>
+      <c r="H19" s="4">
+        <f>COUNTA(H4:H18)</f>
+        <v>7</v>
+      </c>
+      <c r="I19" s="4">
+        <f>COUNTA(I4:I18)</f>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Inplementing final sprint tiles
They had been tested as described in the Excel file.
</commit_message>
<xml_diff>
--- a/Excel/Tile Colection.xlsx
+++ b/Excel/Tile Colection.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="26">
   <si>
     <t>01-Curva-Esq-01</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>BP_Loop-01 Não buga com</t>
+  </si>
+  <si>
+    <t>BP_Curva_Baixo_01</t>
   </si>
 </sst>
 </file>
@@ -507,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I19"/>
+  <dimension ref="B2:I20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,7 +615,7 @@
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
@@ -625,38 +628,30 @@
     </row>
     <row r="8" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="D8" s="8"/>
-      <c r="E8" s="8">
-        <v>1</v>
-      </c>
-      <c r="F8" s="8">
-        <v>3</v>
-      </c>
-      <c r="G8" s="8">
-        <v>1</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="2"/>
       <c r="I8" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="8">
         <v>1</v>
       </c>
       <c r="F9" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G9" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>4</v>
@@ -667,29 +662,33 @@
     </row>
     <row r="10" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
+      <c r="E10" s="8">
+        <v>1</v>
+      </c>
       <c r="F10" s="8">
         <v>1</v>
       </c>
       <c r="G10" s="8">
-        <v>1</v>
-      </c>
-      <c r="H10" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="I10" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G11" s="8">
         <v>1</v>
@@ -701,14 +700,16 @@
     </row>
     <row r="12" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D12" s="8"/>
-      <c r="E12" s="8">
-        <v>3</v>
-      </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8">
+        <v>2</v>
+      </c>
+      <c r="G12" s="8">
+        <v>1</v>
+      </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2" t="s">
         <v>4</v>
@@ -716,57 +717,55 @@
     </row>
     <row r="13" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8">
         <v>3</v>
       </c>
-      <c r="D13" s="8">
-        <v>1</v>
-      </c>
-      <c r="E13" s="8">
-        <v>2</v>
-      </c>
-      <c r="F13" s="8">
-        <v>4</v>
-      </c>
-      <c r="G13" s="8">
-        <v>5</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="2"/>
       <c r="I13" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="14" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="8"/>
+        <v>3</v>
+      </c>
+      <c r="D14" s="8">
+        <v>1</v>
+      </c>
       <c r="E14" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F14" s="8">
         <v>4</v>
       </c>
       <c r="G14" s="8">
-        <v>3</v>
-      </c>
-      <c r="H14" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="I14" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="15" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C15" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
+      <c r="E15" s="8">
+        <v>1</v>
+      </c>
       <c r="F15" s="8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G15" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2" t="s">
@@ -775,13 +774,15 @@
     </row>
     <row r="16" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C16" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
+      <c r="F16" s="8">
+        <v>2</v>
+      </c>
       <c r="G16" s="8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2" t="s">
@@ -790,15 +791,13 @@
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
-      <c r="F17" s="8">
-        <v>3</v>
-      </c>
+      <c r="F17" s="8"/>
       <c r="G17" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="2" t="s">
@@ -807,50 +806,67 @@
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C18" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="F18" s="8">
+        <v>3</v>
+      </c>
+      <c r="G18" s="8">
+        <v>1</v>
+      </c>
+      <c r="H18" s="2"/>
       <c r="I18" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="3" t="s">
+      <c r="C19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="4">
-        <f>COUNTA(C4:C18)</f>
-        <v>15</v>
-      </c>
-      <c r="D19" s="9">
-        <f t="shared" ref="D19:F19" si="0">SUM(D4:D18)</f>
+      <c r="C20" s="4">
+        <f>COUNTA(C4:C19)</f>
+        <v>16</v>
+      </c>
+      <c r="D20" s="9">
+        <f t="shared" ref="D20:F20" si="0">SUM(D4:D19)</f>
         <v>7</v>
       </c>
-      <c r="E19" s="9">
+      <c r="E20" s="9">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="F19" s="9">
+      <c r="F20" s="9">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="G19" s="9">
-        <f>SUM(G4:G18)</f>
+      <c r="G20" s="9">
+        <f>SUM(G4:G19)</f>
         <v>20</v>
       </c>
-      <c r="H19" s="4">
-        <f>COUNTA(H4:H18)</f>
+      <c r="H20" s="4">
+        <f>COUNTA(H4:H19)</f>
         <v>7</v>
       </c>
-      <c r="I19" s="4">
-        <f>COUNTA(I4:I18)</f>
-        <v>15</v>
+      <c r="I20" s="4">
+        <f>COUNTA(I4:I19)</f>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rebalance - Até level 07
</commit_message>
<xml_diff>
--- a/Excel/Tile Colection.xlsx
+++ b/Excel/Tile Colection.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Photonic\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Game Design\Unreal Projects\Photonic\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="37">
   <si>
     <t>01-Curva-Esq-01</t>
   </si>
@@ -95,15 +95,9 @@
     <t>BP_Loop-01</t>
   </si>
   <si>
-    <t>BP_Curva_Cima_01</t>
-  </si>
-  <si>
     <t>BP_Loop-01 Não buga com</t>
   </si>
   <si>
-    <t>BP_Curva_Baixo_01</t>
-  </si>
-  <si>
     <t>Tempo minimo gasto na peça [s]</t>
   </si>
   <si>
@@ -120,13 +114,57 @@
   </si>
   <si>
     <t>= valores de output</t>
+  </si>
+  <si>
+    <t>01-Curva_Cima_01</t>
+  </si>
+  <si>
+    <t>lvl 5</t>
+  </si>
+  <si>
+    <t>01-Curva_Baixo_01</t>
+  </si>
+  <si>
+    <t>lvl 6</t>
+  </si>
+  <si>
+    <t>lvl 7</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">BP_Loop-01 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Buga</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> com (pedro)</t>
+    </r>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,6 +190,14 @@
     <font>
       <b/>
       <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -248,7 +294,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -286,6 +332,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -601,29 +651,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:K25"/>
+  <dimension ref="B2:O25"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.7109375" customWidth="1"/>
     <col min="3" max="3" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="3.28515625" customWidth="1"/>
-    <col min="8" max="10" width="10.28515625" customWidth="1"/>
+    <col min="4" max="11" width="3.28515625" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" customWidth="1"/>
+    <col min="13" max="13" width="10" customWidth="1"/>
+    <col min="14" max="14" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D2" s="16" t="s">
         <v>14</v>
       </c>
       <c r="E2" s="17"/>
       <c r="F2" s="17"/>
-      <c r="G2" s="18"/>
-    </row>
-    <row r="3" spans="3:10" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+    </row>
+    <row r="3" spans="3:15" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
@@ -639,365 +695,490 @@
       <c r="G3" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" s="19"/>
+      <c r="L3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J3" s="4" t="s">
+      <c r="N3" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="O3" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="12">
+        <v>1</v>
+      </c>
+      <c r="E4" s="12">
+        <v>1</v>
+      </c>
+      <c r="F4" s="12">
+        <v>1</v>
+      </c>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="M4" s="12">
+        <v>1</v>
+      </c>
+      <c r="N4" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="12">
+        <v>1</v>
+      </c>
+      <c r="E5" s="12">
+        <v>1</v>
+      </c>
+      <c r="F5" s="12">
+        <v>1</v>
+      </c>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="M5" s="12">
         <v>2</v>
       </c>
-      <c r="E4" s="12">
-        <v>2</v>
-      </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="I4" s="12">
-        <v>1</v>
-      </c>
-      <c r="J4" s="12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="12">
-        <v>2</v>
-      </c>
-      <c r="E5" s="12">
-        <v>3</v>
-      </c>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="I5" s="12">
-        <v>2</v>
-      </c>
-      <c r="J5" s="12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N5" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="12">
+        <v>1</v>
+      </c>
+      <c r="E6" s="12">
+        <v>1</v>
+      </c>
+      <c r="F6" s="12">
+        <v>1</v>
+      </c>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="M6" s="12">
         <v>2</v>
       </c>
-      <c r="E6" s="12">
-        <v>3</v>
-      </c>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="I6" s="12">
-        <v>2</v>
-      </c>
-      <c r="J6" s="12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N6" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="O6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
+      <c r="E7" s="12">
+        <v>1</v>
+      </c>
+      <c r="F7" s="12">
+        <v>1</v>
+      </c>
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
-      <c r="I7" s="12">
-        <v>1.5</v>
-      </c>
-      <c r="J7" s="12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12">
+        <v>2.3181818181818179</v>
+      </c>
+      <c r="N7" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
+      <c r="E8" s="12">
+        <v>1</v>
+      </c>
+      <c r="F8" s="12">
+        <v>1</v>
+      </c>
       <c r="G8" s="12"/>
       <c r="H8" s="12"/>
-      <c r="I8" s="12">
-        <v>1.5</v>
-      </c>
-      <c r="J8" s="12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12">
+        <v>2.3181818181818179</v>
+      </c>
+      <c r="N8" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="12"/>
-      <c r="E9" s="12">
-        <v>1</v>
-      </c>
-      <c r="F9" s="12">
-        <v>3</v>
-      </c>
-      <c r="G9" s="12">
-        <v>1</v>
-      </c>
-      <c r="H9" s="12" t="s">
-        <v>4</v>
-      </c>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
       <c r="I9" s="12">
+        <v>1</v>
+      </c>
+      <c r="J9" s="12">
+        <v>1</v>
+      </c>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="M9" s="12">
         <v>2.7</v>
       </c>
-      <c r="J9" s="12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N9" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="O9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D10" s="12"/>
-      <c r="E10" s="12">
-        <v>1</v>
-      </c>
-      <c r="F10" s="12">
-        <v>1</v>
-      </c>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
       <c r="G10" s="12">
         <v>2</v>
       </c>
-      <c r="H10" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="I10" s="12">
+      <c r="H10" s="12">
+        <v>4</v>
+      </c>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12">
+        <v>1</v>
+      </c>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="M10" s="12">
         <v>2.7</v>
       </c>
-      <c r="J10" s="12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N10" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="12"/>
-      <c r="F11" s="12">
-        <v>1</v>
-      </c>
+      <c r="F11" s="12"/>
       <c r="G11" s="12">
-        <v>1</v>
-      </c>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12">
+        <v>2</v>
+      </c>
+      <c r="H11" s="12">
+        <v>4</v>
+      </c>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12">
+        <v>1</v>
+      </c>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12">
         <v>2.7</v>
       </c>
-      <c r="J11" s="12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N11" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="12"/>
-      <c r="F12" s="12">
-        <v>2</v>
-      </c>
-      <c r="G12" s="12">
-        <v>1</v>
-      </c>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
       <c r="H12" s="12"/>
-      <c r="I12" s="12">
+      <c r="I12" s="12"/>
+      <c r="J12" s="12">
+        <v>1</v>
+      </c>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12">
         <v>2.7</v>
       </c>
-      <c r="J12" s="12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N12" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="O12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D13" s="12"/>
-      <c r="E13" s="12">
-        <v>3</v>
-      </c>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12">
+        <v>1</v>
+      </c>
+      <c r="G13" s="12">
+        <v>1</v>
+      </c>
       <c r="H13" s="12"/>
-      <c r="I13" s="12">
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12">
         <v>3.3</v>
       </c>
-      <c r="J13" s="12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N13" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="12">
-        <v>1</v>
-      </c>
-      <c r="E14" s="12">
-        <v>2</v>
-      </c>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
       <c r="F14" s="12">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G14" s="12">
-        <v>5</v>
-      </c>
-      <c r="H14" s="12" t="s">
-        <v>4</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="H14" s="12"/>
       <c r="I14" s="12">
+        <v>1</v>
+      </c>
+      <c r="J14" s="12">
+        <v>1</v>
+      </c>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="M14" s="12">
         <v>1.2</v>
       </c>
-      <c r="J14" s="12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N14" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C15" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D15" s="12"/>
-      <c r="E15" s="12">
-        <v>1</v>
-      </c>
-      <c r="F15" s="12">
-        <v>4</v>
-      </c>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
       <c r="G15" s="12">
         <v>3</v>
       </c>
       <c r="H15" s="12"/>
       <c r="I15" s="12">
+        <v>1</v>
+      </c>
+      <c r="J15" s="12">
+        <v>1</v>
+      </c>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12">
         <v>1.2</v>
       </c>
-      <c r="J15" s="12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N15" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C16" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="12"/>
-      <c r="F16" s="12">
-        <v>2</v>
-      </c>
-      <c r="G16" s="12">
-        <v>4</v>
-      </c>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
       <c r="H16" s="12"/>
       <c r="I16" s="12">
+        <v>1</v>
+      </c>
+      <c r="J16" s="12">
         <v>2</v>
       </c>
-      <c r="J16" s="12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12">
+        <v>2</v>
+      </c>
+      <c r="N16" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="O16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
-      <c r="G17" s="12">
-        <v>2</v>
-      </c>
+      <c r="G17" s="12"/>
       <c r="H17" s="12"/>
       <c r="I17" s="12">
+        <v>1</v>
+      </c>
+      <c r="J17" s="12">
+        <v>3</v>
+      </c>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12">
         <v>2</v>
       </c>
-      <c r="J17" s="12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="N17" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C18" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="12"/>
-      <c r="F18" s="12">
-        <v>3</v>
-      </c>
+      <c r="F18" s="12"/>
       <c r="G18" s="12">
-        <v>1</v>
-      </c>
-      <c r="H18" s="12"/>
+        <v>2</v>
+      </c>
+      <c r="H18" s="12">
+        <v>2</v>
+      </c>
       <c r="I18" s="12">
+        <v>1</v>
+      </c>
+      <c r="J18" s="12">
+        <v>2</v>
+      </c>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="12">
         <v>3.3</v>
       </c>
-      <c r="J18" s="12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="N18" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C19" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="I19" s="12">
+      <c r="F19" s="12">
+        <v>1</v>
+      </c>
+      <c r="G19" s="12">
+        <v>1</v>
+      </c>
+      <c r="H19" s="12">
+        <v>1</v>
+      </c>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="M19" s="12">
         <v>6.2</v>
       </c>
-      <c r="J19" s="12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="N19" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C20" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D20" s="11">
+        <v>25</v>
+      </c>
+      <c r="E20" s="11">
+        <v>25</v>
+      </c>
+      <c r="F20" s="11">
+        <v>28</v>
+      </c>
+      <c r="G20" s="11">
+        <v>33</v>
+      </c>
+      <c r="H20" s="11">
         <v>30</v>
       </c>
-      <c r="E20" s="11">
+      <c r="I20" s="11">
+        <v>26</v>
+      </c>
+      <c r="J20" s="11">
         <v>50</v>
       </c>
-      <c r="F20" s="11">
-        <v>50</v>
-      </c>
-      <c r="G20" s="11">
-        <v>50</v>
-      </c>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K20" s="11"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
         <v>15</v>
       </c>
@@ -1006,78 +1187,104 @@
         <v>16</v>
       </c>
       <c r="D21" s="5">
-        <f t="shared" ref="D21:F21" si="0">SUM(D4:D19)</f>
-        <v>7</v>
+        <f t="shared" ref="D21:H21" si="0">SUM(D4:D19)</f>
+        <v>3</v>
       </c>
       <c r="E21" s="5">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="F21" s="5">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G21" s="5">
-        <f>SUM(G4:G19)</f>
-        <v>20</v>
+        <f t="shared" si="0"/>
+        <v>14</v>
       </c>
       <c r="H21" s="5">
-        <f>COUNTA(H4:H19)</f>
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="I21" s="5">
+        <f>SUM(I4:I19)</f>
+        <v>6</v>
+      </c>
+      <c r="J21" s="5">
+        <f>SUM(J4:J19)</f>
+        <v>13</v>
+      </c>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5">
+        <f>COUNTA(L4:L19)</f>
         <v>7</v>
       </c>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5">
-        <f>COUNTA(J4:J19)</f>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5">
+        <f>COUNTA(N4:N19)</f>
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B22" s="7"/>
       <c r="C22" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="10">
+        <f>(D4*$M$4+D5*$M$5+D6*$M$6+D7*$M$7+D8*$M$8+D9*$M$9+D10*$M$10+D11*$M$11+D12*$M$12+D13*$M$13+D14*$M$14+D15*$M$15+D16*$M$16+D17*$M$17+D18*$M$18+D19*$M$19+5)/D21*D20</f>
+        <v>83.333333333333343</v>
+      </c>
+      <c r="E22" s="10">
+        <f>(E4*$M$4+E5*$M$5+E6*$M$6+E7*$M$7+E8*$M$8+E9*$M$9+E10*$M$10+E11*$M$11+E12*$M$12+E13*$M$13+E14*$M$14+E15*$M$15+E16*$M$16+E17*$M$17+E18*$M$18+E19*$M$19+5)/E21*E20</f>
+        <v>73.181818181818187</v>
+      </c>
+      <c r="F22" s="10">
+        <f>(F4*$M$4+F5*$M$5+F6*$M$6+F7*$M$7+F8*$M$8+F9*$M$9+F10*$M$10+F11*$M$11+F12*$M$12+F13*$M$13+F14*$M$14+F15*$M$15+F16*$M$16+F17*$M$17+F18*$M$18+F19*$M$19+5)/F21*F20</f>
+        <v>88.677272727272722</v>
+      </c>
+      <c r="G22" s="10">
+        <f>(G4*$M$4+G5*$M$5+G6*$M$6+G7*$M$7+G8*$M$8+G9*$M$9+G10*$M$10+G11*$M$11+G12*$M$12+G13*$M$13+G14*$M$14+G15*$M$15+G16*$M$16+G17*$M$17+G18*$M$18+G19*$M$19+5)/G21*G20</f>
+        <v>92.164285714285739</v>
+      </c>
+      <c r="H22" s="10">
+        <f>(H4*$M$4+H5*$M$5+H6*$M$6+H7*$M$7+H8*$M$8+H9*$M$9+H10*$M$10+H11*$M$11+H12*$M$12+H13*$M$13+H14*$M$14+H15*$M$15+H16*$M$16+H17*$M$17+H18*$M$18+H19*$M$19+5)/H21*H20</f>
+        <v>107.45454545454547</v>
+      </c>
+      <c r="I22" s="10">
+        <f>(I4*$M$4+I5*$M$5+I6*$M$6+I7*$M$7+I8*$M$8+I9*$M$9+I10*$M$10+I11*$M$11+I12*$M$12+I13*$M$13+I14*$M$14+I15*$M$15+I16*$M$16+I17*$M$17+I18*$M$18+I19*$M$19+5)/I21*I20</f>
+        <v>75.400000000000006</v>
+      </c>
+      <c r="J22" s="10">
+        <f>(J4*$M$4+J5*$M$5+J6*$M$6+J7*$M$7+J8*$M$8+J9*$M$9+J10*$M$10+J11*$M$11+J12*$M$12+J13*$M$13+J14*$M$14+J15*$M$15+J16*$M$16+J17*$M$17+J18*$M$18+J19*$M$19+5)/J21*J20</f>
+        <v>133.84615384615384</v>
+      </c>
+      <c r="K22" s="21"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="L23" t="s">
         <v>28</v>
       </c>
-      <c r="D22" s="10">
-        <f>(D4*$I$4+D5*$I$5+D6*$I$6+D7*$I$7+D8*$I$8+D9*$I$9+D10*$I$10+D11*$I$11+D12*$I$12+D13*$I$13+D14*$I$14+D15*$I$15+D16*$I$16+D17*$I$17+D18*$I$18+D19*$I$19+5)/D21*D20</f>
-        <v>69.428571428571416</v>
-      </c>
-      <c r="E22" s="10">
-        <f>(E4*$I$4+E5*$I$5+E6*$I$6+E7*$I$7+E8*$I$8+E9*$I$9+E10*$I$10+E11*$I$11+E12*$I$12+E13*$I$13+E14*$I$14+E15*$I$15+E16*$I$16+E17*$I$17+E18*$I$18+E19*$I$19+5)/E21*E20</f>
-        <v>118.4375</v>
-      </c>
-      <c r="F22" s="10">
-        <f>(F4*$I$4+F5*$I$5+F6*$I$6+F7*$I$7+F8*$I$8+F9*$I$9+F10*$I$10+F11*$I$11+F12*$I$12+F13*$I$13+F14*$I$14+F15*$I$15+F16*$I$16+F17*$I$17+F18*$I$18+F19*$I$19+5)/F21*F20</f>
-        <v>118.5</v>
-      </c>
-      <c r="G22" s="10">
-        <f>(G4*$I$4+G5*$I$5+G6*$I$6+G7*$I$7+G8*$I$8+G9*$I$9+G10*$I$10+G11*$I$11+G12*$I$12+G13*$I$13+G14*$I$14+G15*$I$15+G16*$I$16+G17*$I$17+G18*$I$18+G19*$I$19+5)/G21*G20</f>
-        <v>108.5</v>
-      </c>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="H23" t="s">
-        <v>30</v>
-      </c>
-      <c r="K23" t="str">
-        <f>SUM(D22:G22)/60&amp;" min de jogo"</f>
-        <v>6,91443452380952 min de jogo</v>
-      </c>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="H24" s="13"/>
-      <c r="I24" s="14" t="s">
+      <c r="O23" t="str">
+        <f>SUM(D22:I22)/60&amp;" min de jogo"</f>
+        <v>8.67018759018759 min de jogo</v>
+      </c>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="L24" s="13"/>
+      <c r="M24" s="14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="L25" s="15"/>
+      <c r="M25" s="14" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="H25" s="15"/>
-      <c r="I25" s="14" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Rebalanced lvl 04, fix Victory Menu
</commit_message>
<xml_diff>
--- a/Excel/Tile Colection.xlsx
+++ b/Excel/Tile Colection.xlsx
@@ -653,8 +653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:O25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -923,7 +923,9 @@
       <c r="H11" s="12">
         <v>4</v>
       </c>
-      <c r="I11" s="12"/>
+      <c r="I11" s="12">
+        <v>1</v>
+      </c>
       <c r="J11" s="12">
         <v>1</v>
       </c>
@@ -1208,7 +1210,7 @@
       </c>
       <c r="I21" s="5">
         <f>SUM(I4:I19)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J21" s="5">
         <f>SUM(J4:J19)</f>
@@ -1231,31 +1233,31 @@
         <v>26</v>
       </c>
       <c r="D22" s="10">
-        <f>(D4*$M$4+D5*$M$5+D6*$M$6+D7*$M$7+D8*$M$8+D9*$M$9+D10*$M$10+D11*$M$11+D12*$M$12+D13*$M$13+D14*$M$14+D15*$M$15+D16*$M$16+D17*$M$17+D18*$M$18+D19*$M$19+5)/D21*D20</f>
+        <f t="shared" ref="D22:J22" si="1">(D4*$M$4+D5*$M$5+D6*$M$6+D7*$M$7+D8*$M$8+D9*$M$9+D10*$M$10+D11*$M$11+D12*$M$12+D13*$M$13+D14*$M$14+D15*$M$15+D16*$M$16+D17*$M$17+D18*$M$18+D19*$M$19+5)/D21*D20</f>
         <v>83.333333333333343</v>
       </c>
       <c r="E22" s="10">
-        <f>(E4*$M$4+E5*$M$5+E6*$M$6+E7*$M$7+E8*$M$8+E9*$M$9+E10*$M$10+E11*$M$11+E12*$M$12+E13*$M$13+E14*$M$14+E15*$M$15+E16*$M$16+E17*$M$17+E18*$M$18+E19*$M$19+5)/E21*E20</f>
+        <f t="shared" si="1"/>
         <v>73.181818181818187</v>
       </c>
       <c r="F22" s="10">
-        <f>(F4*$M$4+F5*$M$5+F6*$M$6+F7*$M$7+F8*$M$8+F9*$M$9+F10*$M$10+F11*$M$11+F12*$M$12+F13*$M$13+F14*$M$14+F15*$M$15+F16*$M$16+F17*$M$17+F18*$M$18+F19*$M$19+5)/F21*F20</f>
+        <f t="shared" si="1"/>
         <v>88.677272727272722</v>
       </c>
       <c r="G22" s="10">
-        <f>(G4*$M$4+G5*$M$5+G6*$M$6+G7*$M$7+G8*$M$8+G9*$M$9+G10*$M$10+G11*$M$11+G12*$M$12+G13*$M$13+G14*$M$14+G15*$M$15+G16*$M$16+G17*$M$17+G18*$M$18+G19*$M$19+5)/G21*G20</f>
+        <f t="shared" si="1"/>
         <v>92.164285714285739</v>
       </c>
       <c r="H22" s="10">
-        <f>(H4*$M$4+H5*$M$5+H6*$M$6+H7*$M$7+H8*$M$8+H9*$M$9+H10*$M$10+H11*$M$11+H12*$M$12+H13*$M$13+H14*$M$14+H15*$M$15+H16*$M$16+H17*$M$17+H18*$M$18+H19*$M$19+5)/H21*H20</f>
+        <f t="shared" si="1"/>
         <v>107.45454545454547</v>
       </c>
       <c r="I22" s="10">
-        <f>(I4*$M$4+I5*$M$5+I6*$M$6+I7*$M$7+I8*$M$8+I9*$M$9+I10*$M$10+I11*$M$11+I12*$M$12+I13*$M$13+I14*$M$14+I15*$M$15+I16*$M$16+I17*$M$17+I18*$M$18+I19*$M$19+5)/I21*I20</f>
-        <v>75.400000000000006</v>
+        <f t="shared" si="1"/>
+        <v>74.657142857142858</v>
       </c>
       <c r="J22" s="10">
-        <f>(J4*$M$4+J5*$M$5+J6*$M$6+J7*$M$7+J8*$M$8+J9*$M$9+J10*$M$10+J11*$M$11+J12*$M$12+J13*$M$13+J14*$M$14+J15*$M$15+J16*$M$16+J17*$M$17+J18*$M$18+J19*$M$19+5)/J21*J20</f>
+        <f t="shared" si="1"/>
         <v>133.84615384615384</v>
       </c>
       <c r="K22" s="21"/>
@@ -1268,7 +1270,7 @@
       </c>
       <c r="O23" t="str">
         <f>SUM(D22:I22)/60&amp;" min de jogo"</f>
-        <v>8.67018759018759 min de jogo</v>
+        <v>8.65780663780664 min de jogo</v>
       </c>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">

</xml_diff>